<commit_message>
Melhor documentação e mais gráficos
</commit_message>
<xml_diff>
--- a/DFs-MRV-Limpo.xlsx
+++ b/DFs-MRV-Limpo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\7Periodo\Fin_I\APS1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\INSPER\Engenharia\7-Semestre\Financas-I\APS\Analise-MRV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B6A1AD-296A-480C-B014-FAC5CA883395}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E524B2AE-8DC4-4FA2-938A-BA545037AACD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4AED71FF-91D9-491B-A893-2F3A98F1C88C}"/>
+    <workbookView xWindow="1830" yWindow="1830" windowWidth="17280" windowHeight="8994" activeTab="1" xr2:uid="{4AED71FF-91D9-491B-A893-2F3A98F1C88C}"/>
   </bookViews>
   <sheets>
     <sheet name="BP" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
   <si>
     <t>MRV ON (R$ em milhares)</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Ativo Circulante</t>
   </si>
   <si>
-    <t>Estoques</t>
-  </si>
-  <si>
     <t>Impostos a Recuperar</t>
   </si>
   <si>
@@ -65,24 +62,12 @@
     <t>Ativo Não Circulante</t>
   </si>
   <si>
-    <t>Despesas Antecipadas</t>
-  </si>
-  <si>
-    <t>Contas a Receber</t>
-  </si>
-  <si>
     <t>A Receber de Partes Relacionadas</t>
   </si>
   <si>
     <t>Intangível</t>
   </si>
   <si>
-    <t>Outros</t>
-  </si>
-  <si>
-    <t>Passivo</t>
-  </si>
-  <si>
     <t>Passivo Circulante</t>
   </si>
   <si>
@@ -101,18 +86,6 @@
     <t>Impostos a Pagar</t>
   </si>
   <si>
-    <t>Financiamento</t>
-  </si>
-  <si>
-    <t>Debêntures</t>
-  </si>
-  <si>
-    <t>Outras Obrigações</t>
-  </si>
-  <si>
-    <t>Provisões</t>
-  </si>
-  <si>
     <t>Passivo Não Circulante</t>
   </si>
   <si>
@@ -273,6 +246,57 @@
   </si>
   <si>
     <t>Caixa Gerado Outros Financiamentos</t>
+  </si>
+  <si>
+    <t>Contas a Receber CP</t>
+  </si>
+  <si>
+    <t>Estoques CP</t>
+  </si>
+  <si>
+    <t>Despesas Antecipadas CP</t>
+  </si>
+  <si>
+    <t>Outros CP</t>
+  </si>
+  <si>
+    <t>Contas a Receber LP</t>
+  </si>
+  <si>
+    <t>Estoques LP</t>
+  </si>
+  <si>
+    <t>Despesas Antecipadas LP</t>
+  </si>
+  <si>
+    <t>Outros LP</t>
+  </si>
+  <si>
+    <t>Financiamento CP</t>
+  </si>
+  <si>
+    <t>Debêntures CP</t>
+  </si>
+  <si>
+    <t>Provisões CP</t>
+  </si>
+  <si>
+    <t>Outras Obrigações CP</t>
+  </si>
+  <si>
+    <t>Financiamento LP</t>
+  </si>
+  <si>
+    <t>Debêntures LP</t>
+  </si>
+  <si>
+    <t>Outras Obrigações LP</t>
+  </si>
+  <si>
+    <t>Provisões LP</t>
+  </si>
+  <si>
+    <t>Passivo Total</t>
   </si>
 </sst>
 </file>
@@ -485,7 +509,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -784,17 +808,17 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.88671875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="32.3125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.89453125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -814,7 +838,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -834,7 +858,7 @@
         <v>18062015</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -854,9 +878,9 @@
         <v>8564095</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="11">
         <v>1763552</v>
@@ -874,9 +898,9 @@
         <v>1080705</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="10" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="B5" s="11">
         <v>1662025</v>
@@ -895,9 +919,9 @@
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="10" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B6" s="11">
         <v>3076734</v>
@@ -915,9 +939,9 @@
         <v>3741278</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="11">
         <v>229364</v>
@@ -935,9 +959,9 @@
         <v>78280</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="B8" s="11">
         <v>57205</v>
@@ -955,9 +979,9 @@
         <v>100980</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="10" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="B9" s="11">
         <v>331204</v>
@@ -975,9 +999,9 @@
         <v>1719030</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="9">
         <v>5206929</v>
@@ -995,9 +1019,9 @@
         <v>9497920</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="B11" s="11">
         <v>991402</v>
@@ -1016,9 +1040,9 @@
       </c>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="10" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="B12" s="11">
         <v>3058927</v>
@@ -1036,9 +1060,9 @@
         <v>4860581</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="10" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="B13" s="11">
         <v>36050</v>
@@ -1056,9 +1080,9 @@
         <v>50405</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B14" s="11">
         <v>36643</v>
@@ -1076,9 +1100,9 @@
         <v>60123</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="11">
         <v>783477</v>
@@ -1096,9 +1120,9 @@
         <v>1918962</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="11">
         <v>139986</v>
@@ -1116,9 +1140,9 @@
         <v>564393</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B17" s="11">
         <v>86188</v>
@@ -1136,9 +1160,9 @@
         <v>164431</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="10" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B18" s="11">
         <v>74256</v>
@@ -1156,9 +1180,9 @@
         <v>237931</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="B19" s="7">
         <v>6889526</v>
@@ -1176,9 +1200,9 @@
         <v>12027430</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B20" s="9">
         <v>2924359</v>
@@ -1196,9 +1220,9 @@
         <v>3615810</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B21" s="11">
         <v>110068</v>
@@ -1216,9 +1240,9 @@
         <v>142155</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B22" s="11">
         <v>315109</v>
@@ -1236,9 +1260,9 @@
         <v>467929</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="10" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B23" s="11">
         <v>57318</v>
@@ -1256,9 +1280,9 @@
         <v>90477</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="10" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="B24" s="11">
         <v>600865</v>
@@ -1276,9 +1300,9 @@
         <v>318251</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="10" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="B25" s="11">
         <v>336185</v>
@@ -1296,9 +1320,9 @@
         <v>369269</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="10" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="B26" s="11">
         <v>40331</v>
@@ -1316,9 +1340,9 @@
         <v>41647</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="10" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="B27" s="11">
         <v>1464483</v>
@@ -1336,9 +1360,9 @@
         <v>2186082</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="8" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B28" s="9">
         <v>3965167</v>
@@ -1356,9 +1380,9 @@
         <v>8411620</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="10" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="B29" s="11">
         <v>1376590</v>
@@ -1376,9 +1400,9 @@
         <v>1960044</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="10" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="B30" s="11">
         <v>0</v>
@@ -1396,9 +1420,9 @@
         <v>2003967</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="10" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="B31" s="11">
         <v>2351052</v>
@@ -1416,9 +1440,9 @@
         <v>4154479</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="10" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B32" s="11">
         <v>40126</v>
@@ -1436,9 +1460,9 @@
         <v>66734</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="10" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="B33" s="11">
         <v>197399</v>
@@ -1456,9 +1480,9 @@
         <v>226396</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B34" s="7">
         <v>5437487</v>
@@ -1476,9 +1500,9 @@
         <v>6034585</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="10" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B35" s="11">
         <v>253758</v>
@@ -1496,9 +1520,9 @@
         <v>361254</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="10" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B36" s="11">
         <v>4509521</v>
@@ -1516,9 +1540,9 @@
         <v>4609424</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B37" s="11">
         <v>28977</v>
@@ -1536,9 +1560,9 @@
         <v>59502</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B38" s="11">
         <v>645231</v>
@@ -1556,9 +1580,9 @@
         <v>920796</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="10" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B39" s="11">
         <v>0</v>
@@ -1587,17 +1611,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD49F306-CAF3-4637-A099-D438AE3577F0}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="43.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="43.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="11.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1614,9 +1638,9 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="13" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B2" s="14">
         <v>332400</v>
@@ -1631,9 +1655,9 @@
         <v>689934</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="15" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B3" s="16">
         <v>1053428</v>
@@ -1648,9 +1672,9 @@
         <v>1237169</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="17" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B4" s="18">
         <v>700024</v>
@@ -1665,9 +1689,9 @@
         <v>620992</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="17" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B5" s="18">
         <v>49186</v>
@@ -1682,9 +1706,9 @@
         <v>109731</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="17" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B6" s="18">
         <v>0</v>
@@ -1699,9 +1723,9 @@
         <v>-88293</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="17" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B7" s="18">
         <v>9353</v>
@@ -1716,9 +1740,9 @@
         <v>3132</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="17" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B8" s="18">
         <v>33049</v>
@@ -1733,9 +1757,9 @@
         <v>46741</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="17" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B9" s="18">
         <v>-9780</v>
@@ -1750,9 +1774,9 @@
         <v>30320</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="17" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B10" s="18">
         <v>271596</v>
@@ -1767,9 +1791,9 @@
         <v>514546</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="15" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B11" s="16">
         <v>-721028</v>
@@ -1784,9 +1808,9 @@
         <v>94649</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="17" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B12" s="18">
         <v>10789</v>
@@ -1801,9 +1825,9 @@
         <v>-800940</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="17" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B13" s="18">
         <v>-120535</v>
@@ -1818,9 +1842,9 @@
         <v>772063</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B14" s="18">
         <v>-188833</v>
@@ -1835,9 +1859,9 @@
         <v>-160653</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="17" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B15" s="18">
         <v>-10126</v>
@@ -1852,9 +1876,9 @@
         <v>155134</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="17" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B16" s="18">
         <v>17439</v>
@@ -1869,9 +1893,9 @@
         <v>124626</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="17" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B17" s="18">
         <v>-429762</v>
@@ -1886,9 +1910,9 @@
         <v>4419</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="15" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B18" s="16">
         <v>0</v>
@@ -1903,9 +1927,9 @@
         <v>-641884</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="13" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B19" s="14">
         <v>-988534</v>
@@ -1920,9 +1944,9 @@
         <v>-794716</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="15" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B20" s="16">
         <v>-113615</v>
@@ -1937,9 +1961,9 @@
         <v>-637894</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="17" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B21" s="18">
         <v>-38203</v>
@@ -1954,9 +1978,9 @@
         <v>-761306</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="17" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B22" s="18">
         <v>-75412</v>
@@ -1971,9 +1995,9 @@
         <v>-179957</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="17" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B23" s="18">
         <v>0</v>
@@ -1988,9 +2012,9 @@
         <v>303369</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="15" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B24" s="16">
         <v>-811726</v>
@@ -2005,9 +2029,9 @@
         <v>-163628</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="15" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B25" s="16">
         <v>-63193</v>
@@ -2022,9 +2046,9 @@
         <v>6806</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="13" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B26" s="14">
         <v>861322</v>
@@ -2039,9 +2063,9 @@
         <v>511840</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="15" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B27" s="16">
         <v>1068520</v>
@@ -2056,9 +2080,9 @@
         <v>690157</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="17" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B28" s="18">
         <v>3159708</v>
@@ -2073,9 +2097,9 @@
         <v>2492897</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="17" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B29" s="18">
         <v>-2091188</v>
@@ -2090,9 +2114,9 @@
         <v>-1802740</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="15" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B30" s="16">
         <v>-41090</v>
@@ -2107,9 +2131,9 @@
         <v>-26524</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="17" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B31" s="18">
         <v>4615</v>
@@ -2124,9 +2148,9 @@
         <v>-26524</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="17" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B32" s="18">
         <v>-45705</v>
@@ -2141,9 +2165,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="15" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B33" s="16">
         <v>-282390</v>
@@ -2158,9 +2182,9 @@
         <v>-163933</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="15" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B34" s="16">
         <v>116282</v>
@@ -2175,9 +2199,9 @@
         <v>12140</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="13" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B35" s="14">
         <v>0</v>
@@ -2192,9 +2216,9 @@
         <v>-1272</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="19" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B36" s="20">
         <v>205188</v>
@@ -2222,14 +2246,14 @@
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="16" width="8.88671875" style="21"/>
+    <col min="1" max="1" width="34.5234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="11.89453125" customWidth="1"/>
+    <col min="6" max="16" width="8.89453125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2246,9 +2270,9 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="10" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B2" s="11">
         <v>4759888</v>
@@ -2263,9 +2287,9 @@
         <v>6646359</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="10" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B3" s="11">
         <v>3147749</v>
@@ -2280,9 +2304,9 @@
         <v>4772021</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="8" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B4" s="9">
         <v>1612139</v>
@@ -2308,9 +2332,9 @@
       <c r="O4" s="22"/>
       <c r="P4" s="22"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="10" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B5" s="11">
         <v>550298</v>
@@ -2325,9 +2349,9 @@
         <v>649261</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="10" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B6" s="11">
         <v>319719</v>
@@ -2342,9 +2366,9 @@
         <v>433410</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="10" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B7" s="11">
         <v>72927</v>
@@ -2359,9 +2383,9 @@
         <v>98083</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B8" s="11">
         <v>115487</v>
@@ -2376,9 +2400,9 @@
         <v>129274</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="10" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B9" s="11">
         <v>-33049</v>
@@ -2393,9 +2417,9 @@
         <v>-46741</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B10" s="9">
         <v>666513</v>
@@ -2421,9 +2445,9 @@
       <c r="O10" s="22"/>
       <c r="P10" s="22"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B11" s="11">
         <v>283030</v>
@@ -2438,9 +2462,9 @@
         <v>155541</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="10" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B12" s="11">
         <v>144348</v>
@@ -2455,9 +2479,9 @@
         <v>108529</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B13" s="9">
         <v>805195</v>
@@ -2483,9 +2507,9 @@
       <c r="O13" s="22"/>
       <c r="P13" s="22"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="10" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B14" s="11">
         <v>105171</v>
@@ -2500,9 +2524,9 @@
         <v>139755</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B15" s="7">
         <v>700024</v>

</xml_diff>

<commit_message>
Ajustes Indicadores de Mercado
</commit_message>
<xml_diff>
--- a/DFs-MRV-Limpo.xlsx
+++ b/DFs-MRV-Limpo.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luvi/Desktop/Analise-MRV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\INSPER\Engenharia\7-Semestre\Financas-I\APS\Analise-MRV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A03B397-60AE-BB43-80E6-8E49FA7723B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC9EBA8-C620-4BC6-90DF-C02A63C04EA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="3" xr2:uid="{4AED71FF-91D9-491B-A893-2F3A98F1C88C}"/>
+    <workbookView xWindow="3222" yWindow="1716" windowWidth="17280" windowHeight="8994" activeTab="3" xr2:uid="{4AED71FF-91D9-491B-A893-2F3A98F1C88C}"/>
   </bookViews>
   <sheets>
     <sheet name="BP" sheetId="1" r:id="rId1"/>
     <sheet name="DFC" sheetId="2" r:id="rId2"/>
     <sheet name="DRE" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Ações" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,11 +36,62 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={474D2396-3B5A-4D30-AA2F-97EF85D22CF4}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{474D2396-3B5A-4D30-AA2F-97EF85D22CF4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    R$ em milhares</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={0E5F497C-D1FD-43CB-BC62-853A4DF49BB0}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{0E5F497C-D1FD-43CB-BC62-853A4DF49BB0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    R$ em milhares</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={F83BD455-CFDB-46B2-BCBD-6E6F4D57F8E2}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{F83BD455-CFDB-46B2-BCBD-6E6F4D57F8E2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    R$ em milhares</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
-  <si>
-    <t>MRV ON (R$ em milhares)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
   <si>
     <t>Ativo Total</t>
   </si>
@@ -298,13 +349,22 @@
   </si>
   <si>
     <t>Passivo Total</t>
+  </si>
+  <si>
+    <t>MRV ON</t>
+  </si>
+  <si>
+    <t>Preço por Ação (Fechamento do Ano)</t>
+  </si>
+  <si>
+    <t>Quantidade de Ações</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +435,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -492,7 +558,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,6 +576,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Pedro Ramos" id="{DE9F4A27-840D-4BF8-8C4C-A2DCB8D43F19}" userId="7ae5f1e2c26af788" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -805,24 +879,46 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2021-03-15T03:58:15.99" personId="{DE9F4A27-840D-4BF8-8C4C-A2DCB8D43F19}" id="{474D2396-3B5A-4D30-AA2F-97EF85D22CF4}">
+    <text>R$ em milhares</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2021-03-15T03:58:15.99" personId="{DE9F4A27-840D-4BF8-8C4C-A2DCB8D43F19}" id="{0E5F497C-D1FD-43CB-BC62-853A4DF49BB0}">
+    <text>R$ em milhares</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2021-03-15T03:58:15.99" personId="{DE9F4A27-840D-4BF8-8C4C-A2DCB8D43F19}" id="{F83BD455-CFDB-46B2-BCBD-6E6F4D57F8E2}">
+    <text>R$ em milhares</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2EB8EF-9E07-481F-986E-67E9360D3EB6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2EB8EF-9E07-481F-986E-67E9360D3EB6}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A18" zoomScale="210" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.83203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="32.3125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.83984375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B1" s="5">
         <v>2016</v>
@@ -840,9 +936,9 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="7">
         <v>12327013</v>
@@ -860,9 +956,9 @@
         <v>18062015</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="9">
         <v>7120084</v>
@@ -880,9 +976,9 @@
         <v>8564095</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="11">
         <v>1763552</v>
@@ -900,9 +996,9 @@
         <v>1080705</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="11">
         <v>1662025</v>
@@ -921,9 +1017,9 @@
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="11">
         <v>3076734</v>
@@ -941,9 +1037,9 @@
         <v>3741278</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="11">
         <v>229364</v>
@@ -961,9 +1057,9 @@
         <v>78280</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="11">
         <v>57205</v>
@@ -981,9 +1077,9 @@
         <v>100980</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="11">
         <v>331204</v>
@@ -1001,9 +1097,9 @@
         <v>1719030</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="9">
         <v>5206929</v>
@@ -1021,9 +1117,9 @@
         <v>9497920</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" s="11">
         <v>991402</v>
@@ -1042,9 +1138,9 @@
       </c>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="11">
         <v>3058927</v>
@@ -1062,9 +1158,9 @@
         <v>4860581</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="11">
         <v>36050</v>
@@ -1082,9 +1178,9 @@
         <v>50405</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="11">
         <v>36643</v>
@@ -1102,9 +1198,9 @@
         <v>60123</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="11">
         <v>783477</v>
@@ -1122,9 +1218,9 @@
         <v>1918962</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="11">
         <v>139986</v>
@@ -1142,9 +1238,9 @@
         <v>564393</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="11">
         <v>86188</v>
@@ -1162,9 +1258,9 @@
         <v>164431</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" s="11">
         <v>74256</v>
@@ -1182,9 +1278,9 @@
         <v>237931</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B19" s="7">
         <v>6889526</v>
@@ -1202,9 +1298,9 @@
         <v>12027430</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="9">
         <v>2924359</v>
@@ -1222,9 +1318,9 @@
         <v>3615810</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" s="11">
         <v>110068</v>
@@ -1242,9 +1338,9 @@
         <v>142155</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" s="11">
         <v>315109</v>
@@ -1262,9 +1358,9 @@
         <v>467929</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="11">
         <v>57318</v>
@@ -1282,9 +1378,9 @@
         <v>90477</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24" s="11">
         <v>600865</v>
@@ -1302,9 +1398,9 @@
         <v>318251</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" s="11">
         <v>336185</v>
@@ -1322,9 +1418,9 @@
         <v>369269</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="11">
         <v>40331</v>
@@ -1342,9 +1438,9 @@
         <v>41647</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" s="11">
         <v>1464483</v>
@@ -1362,9 +1458,9 @@
         <v>2186082</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" s="9">
         <v>3965167</v>
@@ -1382,9 +1478,9 @@
         <v>8411620</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B29" s="11">
         <v>1376590</v>
@@ -1402,9 +1498,9 @@
         <v>1960044</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" s="11">
         <v>0</v>
@@ -1422,9 +1518,9 @@
         <v>2003967</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B31" s="11">
         <v>2351052</v>
@@ -1442,9 +1538,9 @@
         <v>4154479</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" s="11">
         <v>40126</v>
@@ -1462,9 +1558,9 @@
         <v>66734</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B33" s="11">
         <v>197399</v>
@@ -1482,9 +1578,9 @@
         <v>226396</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B34" s="7">
         <v>5437487</v>
@@ -1502,9 +1598,9 @@
         <v>6034585</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="11">
         <v>253758</v>
@@ -1522,9 +1618,9 @@
         <v>361254</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" s="11">
         <v>4509521</v>
@@ -1542,9 +1638,9 @@
         <v>4609424</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37" s="11">
         <v>28977</v>
@@ -1562,9 +1658,9 @@
         <v>59502</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B38" s="11">
         <v>645231</v>
@@ -1582,9 +1678,9 @@
         <v>920796</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B39" s="11">
         <v>0</v>
@@ -1606,26 +1702,25 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD49F306-CAF3-4637-A099-D438AE3577F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD49F306-CAF3-4637-A099-D438AE3577F0}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="222" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="43.47265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="11.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B1" s="5">
         <v>2017</v>
@@ -1640,9 +1735,9 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="14">
         <v>332400</v>
@@ -1657,9 +1752,9 @@
         <v>689934</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="16">
         <v>1053428</v>
@@ -1674,9 +1769,9 @@
         <v>1237169</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="18">
         <v>700024</v>
@@ -1691,9 +1786,9 @@
         <v>620992</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="18">
         <v>49186</v>
@@ -1708,9 +1803,9 @@
         <v>109731</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="18">
         <v>0</v>
@@ -1725,9 +1820,9 @@
         <v>-88293</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="18">
         <v>9353</v>
@@ -1742,9 +1837,9 @@
         <v>3132</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="18">
         <v>33049</v>
@@ -1759,9 +1854,9 @@
         <v>46741</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="18">
         <v>-9780</v>
@@ -1776,9 +1871,9 @@
         <v>30320</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="18">
         <v>271596</v>
@@ -1793,9 +1888,9 @@
         <v>514546</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="16">
         <v>-721028</v>
@@ -1810,9 +1905,9 @@
         <v>94649</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="18">
         <v>10789</v>
@@ -1827,9 +1922,9 @@
         <v>-800940</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="18">
         <v>-120535</v>
@@ -1844,9 +1939,9 @@
         <v>772063</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="18">
         <v>-188833</v>
@@ -1861,9 +1956,9 @@
         <v>-160653</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="18">
         <v>-10126</v>
@@ -1878,9 +1973,9 @@
         <v>155134</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="18">
         <v>17439</v>
@@ -1895,9 +1990,9 @@
         <v>124626</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="18">
         <v>-429762</v>
@@ -1912,9 +2007,9 @@
         <v>4419</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="16">
         <v>0</v>
@@ -1929,9 +2024,9 @@
         <v>-641884</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="14">
         <v>-988534</v>
@@ -1946,9 +2041,9 @@
         <v>-794716</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="16">
         <v>-113615</v>
@@ -1963,9 +2058,9 @@
         <v>-637894</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="18">
         <v>-38203</v>
@@ -1980,9 +2075,9 @@
         <v>-761306</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="18">
         <v>-75412</v>
@@ -1997,9 +2092,9 @@
         <v>-179957</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="18">
         <v>0</v>
@@ -2014,9 +2109,9 @@
         <v>303369</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="16">
         <v>-811726</v>
@@ -2031,9 +2126,9 @@
         <v>-163628</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="16">
         <v>-63193</v>
@@ -2048,9 +2143,9 @@
         <v>6806</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="14">
         <v>861322</v>
@@ -2065,9 +2160,9 @@
         <v>511840</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="16">
         <v>1068520</v>
@@ -2082,9 +2177,9 @@
         <v>690157</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" s="18">
         <v>3159708</v>
@@ -2099,9 +2194,9 @@
         <v>2492897</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="18">
         <v>-2091188</v>
@@ -2116,9 +2211,9 @@
         <v>-1802740</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" s="16">
         <v>-41090</v>
@@ -2133,9 +2228,9 @@
         <v>-26524</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31" s="18">
         <v>4615</v>
@@ -2150,9 +2245,9 @@
         <v>-26524</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B32" s="18">
         <v>-45705</v>
@@ -2167,9 +2262,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B33" s="16">
         <v>-282390</v>
@@ -2184,9 +2279,9 @@
         <v>-163933</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B34" s="16">
         <v>116282</v>
@@ -2201,9 +2296,9 @@
         <v>12140</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" s="14">
         <v>0</v>
@@ -2218,9 +2313,9 @@
         <v>-1272</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="20">
         <v>205188</v>
@@ -2237,27 +2332,28 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3FD37F-98C5-40E3-B1ED-6BEB19E70B1C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3FD37F-98C5-40E3-B1ED-6BEB19E70B1C}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="184" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="11.83203125" customWidth="1"/>
-    <col min="6" max="16" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="34.47265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="11.83984375" customWidth="1"/>
+    <col min="6" max="16" width="8.83984375" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B1" s="5">
         <v>2017</v>
@@ -2272,9 +2368,9 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="11">
         <v>4759888</v>
@@ -2289,9 +2385,9 @@
         <v>6646359</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="11">
         <v>3147749</v>
@@ -2306,9 +2402,9 @@
         <v>4772021</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="9">
         <v>1612139</v>
@@ -2334,9 +2430,9 @@
       <c r="O4" s="22"/>
       <c r="P4" s="22"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="11">
         <v>550298</v>
@@ -2351,9 +2447,9 @@
         <v>649261</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="11">
         <v>319719</v>
@@ -2368,9 +2464,9 @@
         <v>433410</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="11">
         <v>72927</v>
@@ -2385,9 +2481,9 @@
         <v>98083</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="11">
         <v>115487</v>
@@ -2402,9 +2498,9 @@
         <v>129274</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="11">
         <v>-33049</v>
@@ -2419,9 +2515,9 @@
         <v>-46741</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="9">
         <v>666513</v>
@@ -2447,9 +2543,9 @@
       <c r="O10" s="22"/>
       <c r="P10" s="22"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="11">
         <v>283030</v>
@@ -2464,9 +2560,9 @@
         <v>155541</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="11">
         <v>144348</v>
@@ -2481,9 +2577,9 @@
         <v>108529</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="9">
         <v>805195</v>
@@ -2509,9 +2605,9 @@
       <c r="O13" s="22"/>
       <c r="P13" s="22"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="11">
         <v>105171</v>
@@ -2526,9 +2622,9 @@
         <v>139755</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="7">
         <v>700024</v>
@@ -2558,76 +2654,223 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2EDE1F-0CA5-454F-B36A-E70AF3985794}">
-  <dimension ref="A5:E9"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="34.47265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="11.83984375" customWidth="1"/>
+    <col min="6" max="16" width="8.83984375" style="21"/>
+  </cols>
   <sheetData>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="5">
         <v>2017</v>
       </c>
-      <c r="B5">
+      <c r="C1" s="5">
         <v>2018</v>
       </c>
-      <c r="C5">
+      <c r="D1" s="5">
         <v>2019</v>
       </c>
-      <c r="D5">
+      <c r="E1" s="5">
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="23">
-        <f>DRE!B15</f>
-        <v>700024</v>
-      </c>
-      <c r="B6" s="23">
-        <f>DRE!C15</f>
-        <v>758137</v>
-      </c>
-      <c r="C6" s="23">
-        <f>DRE!D15</f>
-        <v>747876</v>
-      </c>
-      <c r="D6" s="23">
-        <f>DRE!E15</f>
-        <v>620992</v>
-      </c>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <f>A6/A9</f>
-        <v>472989.18918918917</v>
-      </c>
-      <c r="B7">
-        <f t="shared" ref="B7:C7" si="0">B6/B9</f>
-        <v>443354.97076023393</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>445164.28571428574</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1.48</v>
-      </c>
-      <c r="B9">
-        <v>1.71</v>
-      </c>
-      <c r="C9">
-        <v>1.68</v>
-      </c>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="23">
+        <v>10.619189782999999</v>
+      </c>
+      <c r="C2" s="23">
+        <v>11.268418542999999</v>
+      </c>
+      <c r="D2" s="23">
+        <v>20.921103453000001</v>
+      </c>
+      <c r="E2" s="23">
+        <v>18.754560669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="11">
+        <v>441848</v>
+      </c>
+      <c r="C3" s="11">
+        <v>441011</v>
+      </c>
+      <c r="D3" s="11">
+        <v>443821</v>
+      </c>
+      <c r="E3" s="11">
+        <v>481953</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+    </row>
+    <row r="10" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+    </row>
+    <row r="13" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+    </row>
+    <row r="15" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>